<commit_message>
+feladat bejegyzés: nem regisztrált felhasználók oldala, lekérdezése
</commit_message>
<xml_diff>
--- a/EB_projekt_menet.xlsx
+++ b/EB_projekt_menet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://plkik.sharepoint.com/sites/Esti_projektmunka_gyakorloter/Megosztott dokumentumok/General/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1F698BC9-BE54-4A87-A5EB-F9267542A308}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{074AB47C-0AA8-4ECD-BE9B-9B4991025080}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16120" xr2:uid="{39ABA147-C24E-9C46-B36D-D7DDC8F00C1D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="103">
   <si>
     <t>Projektmunka terv</t>
   </si>
@@ -234,6 +234,12 @@
   </si>
   <si>
     <t>session_start() function</t>
+  </si>
+  <si>
+    <t>nem regisztrált felhasználók oldalának elkészítése</t>
+  </si>
+  <si>
+    <t>nem regisztrált felhasználók keresési felülete</t>
   </si>
   <si>
     <t>4. adományozás és menhely infók</t>
@@ -1300,10 +1306,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B8E7F18-5A48-1C46-BD03-BEEDB5094022}">
-  <dimension ref="B1:I96"/>
+  <dimension ref="B1:I98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B40" workbookViewId="0">
-      <selection activeCell="C68" sqref="C68"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="G60" sqref="G60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -1368,7 +1374,7 @@
         <v>44591</v>
       </c>
       <c r="E3" s="7">
-        <f t="shared" ref="E3:E91" si="0">F3-D3</f>
+        <f t="shared" ref="E3:E93" si="0">F3-D3</f>
         <v>7</v>
       </c>
       <c r="F3" s="8">
@@ -2333,61 +2339,55 @@
       </c>
       <c r="I58" s="10"/>
     </row>
-    <row r="59" spans="2:9" s="26" customFormat="1" ht="18.75">
-      <c r="B59" s="33" t="s">
+    <row r="59" spans="2:9" ht="18.75">
+      <c r="B59" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="C59" s="20" t="s">
+      <c r="C59" s="5"/>
+      <c r="D59" s="6">
+        <v>44591</v>
+      </c>
+      <c r="E59" s="7"/>
+      <c r="F59" s="14"/>
+      <c r="G59" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="H59" s="30"/>
+      <c r="I59" s="10"/>
+    </row>
+    <row r="60" spans="2:9" ht="18.75">
+      <c r="B60" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="C60" s="5"/>
+      <c r="D60" s="6">
+        <v>44591</v>
+      </c>
+      <c r="E60" s="7"/>
+      <c r="F60" s="14"/>
+      <c r="G60" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="H60" s="30"/>
+      <c r="I60" s="10"/>
+    </row>
+    <row r="61" spans="2:9" s="26" customFormat="1" ht="18.75">
+      <c r="B61" s="33" t="s">
+        <v>67</v>
+      </c>
+      <c r="C61" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="D59" s="21">
-        <v>44591</v>
-      </c>
-      <c r="E59" s="22">
+      <c r="D61" s="21">
+        <v>44591</v>
+      </c>
+      <c r="E61" s="22">
         <f t="shared" si="0"/>
         <v>-44591</v>
       </c>
-      <c r="F59" s="27"/>
-      <c r="G59" s="24" t="s">
+      <c r="F61" s="27"/>
+      <c r="G61" s="24" t="s">
         <v>17</v>
-      </c>
-      <c r="H59" s="30"/>
-      <c r="I59" s="25"/>
-    </row>
-    <row r="60" spans="2:9" s="26" customFormat="1" ht="18.75">
-      <c r="B60" s="34" t="s">
-        <v>66</v>
-      </c>
-      <c r="C60" s="20"/>
-      <c r="D60" s="6">
-        <v>44591</v>
-      </c>
-      <c r="E60" s="7">
-        <f t="shared" si="0"/>
-        <v>-44591</v>
-      </c>
-      <c r="F60" s="20"/>
-      <c r="G60" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="H60" s="30"/>
-      <c r="I60" s="25"/>
-    </row>
-    <row r="61" spans="2:9" s="26" customFormat="1" ht="18.75">
-      <c r="B61" s="34" t="s">
-        <v>67</v>
-      </c>
-      <c r="C61" s="20"/>
-      <c r="D61" s="6">
-        <v>44591</v>
-      </c>
-      <c r="E61" s="7">
-        <f t="shared" si="0"/>
-        <v>-44591</v>
-      </c>
-      <c r="F61" s="20"/>
-      <c r="G61" s="9" t="s">
-        <v>11</v>
       </c>
       <c r="H61" s="30"/>
       <c r="I61" s="25"/>
@@ -2444,14 +2444,14 @@
       </c>
       <c r="F64" s="20"/>
       <c r="G64" s="9" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="H64" s="30"/>
       <c r="I64" s="25"/>
     </row>
     <row r="65" spans="2:9" s="26" customFormat="1" ht="18.75">
-      <c r="B65" s="13" t="s">
-        <v>24</v>
+      <c r="B65" s="34" t="s">
+        <v>71</v>
       </c>
       <c r="C65" s="20"/>
       <c r="D65" s="6">
@@ -2469,8 +2469,8 @@
       <c r="I65" s="25"/>
     </row>
     <row r="66" spans="2:9" s="26" customFormat="1" ht="18.75">
-      <c r="B66" s="13" t="s">
-        <v>26</v>
+      <c r="B66" s="34" t="s">
+        <v>72</v>
       </c>
       <c r="C66" s="20"/>
       <c r="D66" s="6">
@@ -2482,14 +2482,14 @@
       </c>
       <c r="F66" s="20"/>
       <c r="G66" s="9" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="H66" s="30"/>
       <c r="I66" s="25"/>
     </row>
     <row r="67" spans="2:9" s="26" customFormat="1" ht="18.75">
       <c r="B67" s="13" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C67" s="20"/>
       <c r="D67" s="6">
@@ -2506,104 +2506,95 @@
       <c r="H67" s="30"/>
       <c r="I67" s="25"/>
     </row>
-    <row r="68" spans="2:9" ht="18.75">
+    <row r="68" spans="2:9" s="26" customFormat="1" ht="18.75">
       <c r="B68" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="C68" s="5" t="s">
-        <v>10</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="C68" s="20"/>
       <c r="D68" s="6">
         <v>44591</v>
       </c>
       <c r="E68" s="7">
         <f t="shared" si="0"/>
-        <v>49</v>
-      </c>
-      <c r="F68" s="8">
-        <v>44640</v>
-      </c>
+        <v>-44591</v>
+      </c>
+      <c r="F68" s="20"/>
       <c r="G68" s="9" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="H68" s="30"/>
-      <c r="I68" s="10" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="69" spans="2:9" s="26" customFormat="1" ht="23.25">
-      <c r="B69" s="19" t="s">
-        <v>72</v>
-      </c>
-      <c r="C69" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="D69" s="21">
-        <v>44591</v>
-      </c>
-      <c r="E69" s="22">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="F69" s="23">
-        <v>44592</v>
-      </c>
-      <c r="G69" s="24" t="s">
-        <v>17</v>
-      </c>
-      <c r="H69" s="29"/>
+      <c r="I68" s="25"/>
+    </row>
+    <row r="69" spans="2:9" s="26" customFormat="1" ht="18.75">
+      <c r="B69" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="C69" s="20"/>
+      <c r="D69" s="6">
+        <v>44591</v>
+      </c>
+      <c r="E69" s="7">
+        <f t="shared" si="0"/>
+        <v>-44591</v>
+      </c>
+      <c r="F69" s="20"/>
+      <c r="G69" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="H69" s="30"/>
       <c r="I69" s="25"/>
     </row>
     <row r="70" spans="2:9" ht="18.75">
       <c r="B70" s="13" t="s">
-        <v>73</v>
+        <v>60</v>
       </c>
       <c r="C70" s="5" t="s">
-        <v>46</v>
+        <v>10</v>
       </c>
       <c r="D70" s="6">
         <v>44591</v>
       </c>
       <c r="E70" s="7">
         <f t="shared" si="0"/>
-        <v>16</v>
-      </c>
-      <c r="F70" s="6">
-        <v>44607</v>
+        <v>49</v>
+      </c>
+      <c r="F70" s="8">
+        <v>44640</v>
       </c>
       <c r="G70" s="9" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="H70" s="30"/>
       <c r="I70" s="10" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="71" spans="2:9" s="26" customFormat="1" ht="23.25">
+      <c r="B71" s="19" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="71" spans="2:9" ht="18.75">
-      <c r="B71" s="13" t="s">
-        <v>75</v>
-      </c>
-      <c r="C71" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="D71" s="6">
-        <v>44591</v>
-      </c>
-      <c r="E71" s="7">
-        <f>F71-D71</f>
-        <v>11</v>
-      </c>
-      <c r="F71" s="6">
-        <v>44602</v>
-      </c>
-      <c r="G71" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="H71" s="30"/>
+      <c r="C71" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="D71" s="21">
+        <v>44591</v>
+      </c>
+      <c r="E71" s="22">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F71" s="23">
+        <v>44592</v>
+      </c>
+      <c r="G71" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="H71" s="29"/>
+      <c r="I71" s="25"/>
     </row>
     <row r="72" spans="2:9" ht="18.75">
       <c r="B72" s="13" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C72" s="5" t="s">
         <v>46</v>
@@ -2613,16 +2604,18 @@
       </c>
       <c r="E72" s="7">
         <f t="shared" si="0"/>
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="F72" s="6">
-        <v>44612</v>
+        <v>44607</v>
       </c>
       <c r="G72" s="9" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="H72" s="30"/>
-      <c r="I72" s="10"/>
+      <c r="I72" s="10" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="73" spans="2:9" ht="18.75">
       <c r="B73" s="13" t="s">
@@ -2635,17 +2628,16 @@
         <v>44591</v>
       </c>
       <c r="E73" s="7">
-        <f t="shared" si="0"/>
-        <v>49</v>
+        <f>F73-D73</f>
+        <v>11</v>
       </c>
       <c r="F73" s="6">
-        <v>44640</v>
+        <v>44602</v>
       </c>
       <c r="G73" s="9" t="s">
         <v>14</v>
       </c>
       <c r="H73" s="30"/>
-      <c r="I73" s="10"/>
     </row>
     <row r="74" spans="2:9" ht="18.75">
       <c r="B74" s="13" t="s">
@@ -2659,10 +2651,10 @@
       </c>
       <c r="E74" s="7">
         <f t="shared" si="0"/>
-        <v>43</v>
+        <v>21</v>
       </c>
       <c r="F74" s="6">
-        <v>44634</v>
+        <v>44612</v>
       </c>
       <c r="G74" s="9" t="s">
         <v>14</v>
@@ -2682,10 +2674,10 @@
       </c>
       <c r="E75" s="7">
         <f t="shared" si="0"/>
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="F75" s="6">
-        <v>44634</v>
+        <v>44640</v>
       </c>
       <c r="G75" s="9" t="s">
         <v>14</v>
@@ -2705,10 +2697,10 @@
       </c>
       <c r="E76" s="7">
         <f t="shared" si="0"/>
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F76" s="6">
-        <v>44633</v>
+        <v>44634</v>
       </c>
       <c r="G76" s="9" t="s">
         <v>14</v>
@@ -2717,7 +2709,7 @@
       <c r="I76" s="10"/>
     </row>
     <row r="77" spans="2:9" ht="18.75">
-      <c r="B77" s="35" t="s">
+      <c r="B77" s="13" t="s">
         <v>81</v>
       </c>
       <c r="C77" s="5" t="s">
@@ -2728,19 +2720,19 @@
       </c>
       <c r="E77" s="7">
         <f t="shared" si="0"/>
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="F77" s="6">
-        <v>44638</v>
+        <v>44634</v>
       </c>
       <c r="G77" s="9" t="s">
         <v>14</v>
       </c>
       <c r="H77" s="30"/>
-      <c r="I77" s="16"/>
-    </row>
-    <row r="78" spans="2:9" ht="21" customHeight="1">
-      <c r="B78" s="35" t="s">
+      <c r="I77" s="10"/>
+    </row>
+    <row r="78" spans="2:9" ht="18.75">
+      <c r="B78" s="13" t="s">
         <v>82</v>
       </c>
       <c r="C78" s="5" t="s">
@@ -2751,22 +2743,20 @@
       </c>
       <c r="E78" s="7">
         <f t="shared" si="0"/>
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="F78" s="6">
-        <v>44639</v>
+        <v>44633</v>
       </c>
       <c r="G78" s="9" t="s">
         <v>14</v>
       </c>
       <c r="H78" s="30"/>
-      <c r="I78" s="36" t="s">
+      <c r="I78" s="10"/>
+    </row>
+    <row r="79" spans="2:9" ht="18.75">
+      <c r="B79" s="35" t="s">
         <v>83</v>
-      </c>
-    </row>
-    <row r="79" spans="2:9" ht="18.75">
-      <c r="B79" s="12" t="s">
-        <v>84</v>
       </c>
       <c r="C79" s="5" t="s">
         <v>46</v>
@@ -2776,64 +2766,68 @@
       </c>
       <c r="E79" s="7">
         <f t="shared" si="0"/>
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F79" s="6">
-        <v>44639</v>
+        <v>44638</v>
       </c>
       <c r="G79" s="9" t="s">
         <v>14</v>
       </c>
       <c r="H79" s="30"/>
-      <c r="I79" s="37"/>
-    </row>
-    <row r="80" spans="2:9" ht="37.5">
-      <c r="B80" s="13" t="s">
+      <c r="I79" s="16"/>
+    </row>
+    <row r="80" spans="2:9" ht="21" customHeight="1">
+      <c r="B80" s="35" t="s">
+        <v>84</v>
+      </c>
+      <c r="C80" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D80" s="6">
+        <v>44591</v>
+      </c>
+      <c r="E80" s="7">
+        <f t="shared" si="0"/>
+        <v>48</v>
+      </c>
+      <c r="F80" s="6">
+        <v>44639</v>
+      </c>
+      <c r="G80" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="H80" s="30"/>
+      <c r="I80" s="36" t="s">
         <v>85</v>
       </c>
-      <c r="C80" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D80" s="6">
-        <v>44591</v>
-      </c>
-      <c r="E80" s="7">
-        <f t="shared" si="0"/>
-        <v>-44591</v>
-      </c>
-      <c r="F80" s="6"/>
-      <c r="G80" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="H80" s="30"/>
-      <c r="I80" s="10" t="s">
+    </row>
+    <row r="81" spans="2:9" ht="18.75">
+      <c r="B81" s="12" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="81" spans="2:9" ht="18.75">
-      <c r="B81" s="13" t="s">
+      <c r="C81" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D81" s="6">
+        <v>44591</v>
+      </c>
+      <c r="E81" s="7">
+        <f t="shared" si="0"/>
+        <v>48</v>
+      </c>
+      <c r="F81" s="6">
+        <v>44639</v>
+      </c>
+      <c r="G81" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="H81" s="30"/>
+      <c r="I81" s="37"/>
+    </row>
+    <row r="82" spans="2:9" ht="37.5">
+      <c r="B82" s="13" t="s">
         <v>87</v>
-      </c>
-      <c r="C81" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D81" s="6">
-        <v>44591</v>
-      </c>
-      <c r="E81" s="7">
-        <f t="shared" si="0"/>
-        <v>-44591</v>
-      </c>
-      <c r="F81" s="41"/>
-      <c r="G81" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="H81" s="30"/>
-      <c r="I81" s="10"/>
-    </row>
-    <row r="82" spans="2:9" ht="23.25">
-      <c r="B82" s="18" t="s">
-        <v>88</v>
       </c>
       <c r="C82" s="5" t="s">
         <v>10</v>
@@ -2841,67 +2835,65 @@
       <c r="D82" s="6">
         <v>44591</v>
       </c>
-      <c r="E82" s="39">
-        <f t="shared" si="0"/>
-        <v>29</v>
-      </c>
-      <c r="F82" s="38">
-        <v>44620</v>
-      </c>
-      <c r="G82" s="40" t="s">
-        <v>14</v>
+      <c r="E82" s="7">
+        <f t="shared" si="0"/>
+        <v>-44591</v>
+      </c>
+      <c r="F82" s="6"/>
+      <c r="G82" s="9" t="s">
+        <v>11</v>
       </c>
       <c r="H82" s="30"/>
-      <c r="I82" s="10"/>
+      <c r="I82" s="10" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="83" spans="2:9" ht="18.75">
       <c r="B83" s="13" t="s">
         <v>89</v>
       </c>
       <c r="C83" s="5" t="s">
-        <v>46</v>
+        <v>10</v>
       </c>
       <c r="D83" s="6">
         <v>44591</v>
       </c>
-      <c r="E83" s="39">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="F83" s="38">
-        <v>44592</v>
-      </c>
-      <c r="G83" s="40" t="s">
+      <c r="E83" s="7">
+        <f t="shared" si="0"/>
+        <v>-44591</v>
+      </c>
+      <c r="F83" s="41"/>
+      <c r="G83" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="H83" s="30"/>
+      <c r="I83" s="10"/>
+    </row>
+    <row r="84" spans="2:9" ht="23.25">
+      <c r="B84" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="C84" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D84" s="6">
+        <v>44591</v>
+      </c>
+      <c r="E84" s="39">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="F84" s="38">
+        <v>44620</v>
+      </c>
+      <c r="G84" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="H83" s="31"/>
-      <c r="I83" s="10"/>
-    </row>
-    <row r="84" spans="2:9" ht="18.75">
-      <c r="B84" s="15" t="s">
-        <v>90</v>
-      </c>
-      <c r="C84" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="D84" s="6">
-        <v>44591</v>
-      </c>
-      <c r="E84" s="39">
-        <f t="shared" si="0"/>
-        <v>21</v>
-      </c>
-      <c r="F84" s="38">
-        <v>44612</v>
-      </c>
-      <c r="G84" s="43" t="s">
-        <v>14</v>
-      </c>
-      <c r="H84" s="42"/>
-      <c r="I84" s="44"/>
+      <c r="H84" s="30"/>
+      <c r="I84" s="10"/>
     </row>
     <row r="85" spans="2:9" ht="18.75">
-      <c r="B85" s="15" t="s">
+      <c r="B85" s="13" t="s">
         <v>91</v>
       </c>
       <c r="C85" s="5" t="s">
@@ -2912,39 +2904,43 @@
       </c>
       <c r="E85" s="39">
         <f t="shared" si="0"/>
-        <v>22</v>
+        <v>1</v>
       </c>
       <c r="F85" s="38">
-        <v>44613</v>
-      </c>
-      <c r="G85" s="43"/>
-      <c r="H85" s="42"/>
-      <c r="I85" s="44"/>
+        <v>44592</v>
+      </c>
+      <c r="G85" s="40" t="s">
+        <v>14</v>
+      </c>
+      <c r="H85" s="31"/>
+      <c r="I85" s="10"/>
     </row>
     <row r="86" spans="2:9" ht="18.75">
       <c r="B86" s="15" t="s">
         <v>92</v>
       </c>
       <c r="C86" s="5" t="s">
-        <v>93</v>
+        <v>46</v>
       </c>
       <c r="D86" s="6">
         <v>44591</v>
       </c>
       <c r="E86" s="39">
         <f t="shared" si="0"/>
-        <v>49</v>
+        <v>21</v>
       </c>
       <c r="F86" s="38">
-        <v>44640</v>
-      </c>
-      <c r="G86" s="43"/>
+        <v>44612</v>
+      </c>
+      <c r="G86" s="43" t="s">
+        <v>14</v>
+      </c>
       <c r="H86" s="42"/>
       <c r="I86" s="44"/>
     </row>
     <row r="87" spans="2:9" ht="18.75">
       <c r="B87" s="15" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C87" s="5" t="s">
         <v>46</v>
@@ -2954,33 +2950,33 @@
       </c>
       <c r="E87" s="39">
         <f t="shared" si="0"/>
-        <v>-44591</v>
-      </c>
-      <c r="F87" s="38"/>
-      <c r="G87" s="43" t="s">
-        <v>14</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="F87" s="38">
+        <v>44613</v>
+      </c>
+      <c r="G87" s="43"/>
       <c r="H87" s="42"/>
       <c r="I87" s="44"/>
     </row>
     <row r="88" spans="2:9" ht="18.75">
       <c r="B88" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="C88" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="C88" s="5" t="s">
-        <v>46</v>
-      </c>
       <c r="D88" s="6">
         <v>44591</v>
       </c>
       <c r="E88" s="39">
         <f t="shared" si="0"/>
-        <v>-44591</v>
-      </c>
-      <c r="F88" s="38"/>
-      <c r="G88" s="43" t="s">
-        <v>14</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="F88" s="38">
+        <v>44640</v>
+      </c>
+      <c r="G88" s="43"/>
       <c r="H88" s="42"/>
       <c r="I88" s="44"/>
     </row>
@@ -2989,7 +2985,7 @@
         <v>96</v>
       </c>
       <c r="C89" s="5" t="s">
-        <v>10</v>
+        <v>46</v>
       </c>
       <c r="D89" s="6">
         <v>44591</v>
@@ -3005,53 +3001,95 @@
       <c r="H89" s="42"/>
       <c r="I89" s="44"/>
     </row>
-    <row r="90" spans="2:9" ht="37.5">
+    <row r="90" spans="2:9" ht="18.75">
       <c r="B90" s="15" t="s">
         <v>97</v>
       </c>
-      <c r="C90" s="52" t="s">
+      <c r="C90" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D90" s="6">
+        <v>44591</v>
+      </c>
+      <c r="E90" s="39">
+        <f t="shared" si="0"/>
+        <v>-44591</v>
+      </c>
+      <c r="F90" s="38"/>
+      <c r="G90" s="43" t="s">
+        <v>14</v>
+      </c>
+      <c r="H90" s="42"/>
+      <c r="I90" s="44"/>
+    </row>
+    <row r="91" spans="2:9" ht="18.75">
+      <c r="B91" s="15" t="s">
+        <v>98</v>
+      </c>
+      <c r="C91" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D90" s="41">
-        <v>44591</v>
-      </c>
-      <c r="E90" s="53">
+      <c r="D91" s="6">
+        <v>44591</v>
+      </c>
+      <c r="E91" s="39">
         <f t="shared" si="0"/>
         <v>-44591</v>
       </c>
-      <c r="F90" s="54"/>
-      <c r="G90" s="55" t="s">
+      <c r="F91" s="38"/>
+      <c r="G91" s="43" t="s">
         <v>14</v>
       </c>
-      <c r="H90" s="56"/>
-      <c r="I90" s="44" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="91" spans="2:9" ht="18.75">
-      <c r="B91" s="46"/>
-      <c r="C91" s="47"/>
-      <c r="D91" s="48">
-        <v>44591</v>
-      </c>
-      <c r="E91" s="49">
+      <c r="H91" s="42"/>
+      <c r="I91" s="44"/>
+    </row>
+    <row r="92" spans="2:9" ht="37.5">
+      <c r="B92" s="15" t="s">
+        <v>99</v>
+      </c>
+      <c r="C92" s="52" t="s">
+        <v>10</v>
+      </c>
+      <c r="D92" s="41">
+        <v>44591</v>
+      </c>
+      <c r="E92" s="53">
         <f t="shared" si="0"/>
         <v>-44591</v>
       </c>
-      <c r="F91" s="47"/>
-      <c r="G91" s="50" t="s">
+      <c r="F92" s="54"/>
+      <c r="G92" s="55" t="s">
         <v>14</v>
       </c>
-      <c r="H91" s="51"/>
-      <c r="I91" s="45"/>
-    </row>
-    <row r="96" spans="2:9">
-      <c r="D96" s="17"/>
-      <c r="E96" s="17"/>
+      <c r="H92" s="56"/>
+      <c r="I92" s="44" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="93" spans="2:9" ht="18.75">
+      <c r="B93" s="46"/>
+      <c r="C93" s="47"/>
+      <c r="D93" s="48">
+        <v>44591</v>
+      </c>
+      <c r="E93" s="49">
+        <f t="shared" si="0"/>
+        <v>-44591</v>
+      </c>
+      <c r="F93" s="47"/>
+      <c r="G93" s="50" t="s">
+        <v>14</v>
+      </c>
+      <c r="H93" s="51"/>
+      <c r="I93" s="45"/>
+    </row>
+    <row r="98" spans="4:5">
+      <c r="D98" s="17"/>
+      <c r="E98" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="I78:I79"/>
+    <mergeCell ref="I80:I81"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -3062,7 +3100,7 @@
           <x14:formula1>
             <xm:f>'Háttér adatok'!$C$2:$C$7</xm:f>
           </x14:formula1>
-          <xm:sqref>C2:C91</xm:sqref>
+          <xm:sqref>C2:C93</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -3090,7 +3128,7 @@
     </row>
     <row r="3" spans="3:3">
       <c r="C3" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="4" spans="3:3">
@@ -3100,7 +3138,7 @@
     </row>
     <row r="5" spans="3:3">
       <c r="C5" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
     </row>
     <row r="6" spans="3:3">
@@ -3110,7 +3148,7 @@
     </row>
     <row r="7" spans="3:3">
       <c r="C7" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>

</xml_diff>